<commit_message>
Corrected TOP_INS for solar
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_LandUse_v1.xlsx
+++ b/SuppXLS/Scen_LandUse_v1.xlsx
@@ -8,21 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BSuleimenov\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743A6F0C-F6BC-4320-A557-9F6C095E27A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38849F23-8116-4AC7-8671-834FE32D972A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
-    <sheet name="UPD" sheetId="11" r:id="rId2"/>
-    <sheet name="UCT1" sheetId="1" r:id="rId3"/>
-    <sheet name="UCT2" sheetId="12" r:id="rId4"/>
-    <sheet name="UCT3" sheetId="13" r:id="rId5"/>
-    <sheet name="UCT4" sheetId="14" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -106,44 +97,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Gary Goldstein</author>
-  </authors>
-  <commentList>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="99">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -190,15 +145,9 @@
     <t>UC_Desc</t>
   </si>
   <si>
-    <t>~UC_Sets: R_S: AllRegions</t>
-  </si>
-  <si>
     <t>TimeSlice</t>
   </si>
   <si>
-    <t>AllRegions</t>
-  </si>
-  <si>
     <t>Pset_PD</t>
   </si>
   <si>
@@ -214,40 +163,10 @@
     <t>Val_Cond</t>
   </si>
   <si>
-    <t>~TFM_UPD</t>
-  </si>
-  <si>
     <t>UC - Each Region/Period</t>
   </si>
   <si>
-    <t>~UC_Sets: T_S:</t>
-  </si>
-  <si>
-    <t>UC - Each Region/All Periods</t>
-  </si>
-  <si>
-    <t>UC - All Regions/Each Period</t>
-  </si>
-  <si>
-    <t>UC - All Regions/Periods</t>
-  </si>
-  <si>
-    <t>UC_RHSRTS</t>
-  </si>
-  <si>
-    <t>UC_RHSR</t>
-  </si>
-  <si>
-    <t>UC_RHSTS</t>
-  </si>
-  <si>
-    <t>UC_RHS</t>
-  </si>
-  <si>
     <t>Trans - Insert</t>
-  </si>
-  <si>
-    <t>Trans - Update</t>
   </si>
   <si>
     <t>~TFM_TOPINS</t>
@@ -473,6 +392,21 @@
   </si>
   <si>
     <t>VDA_FLOP</t>
+  </si>
+  <si>
+    <t>ACT_EFF</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>PWRSOL</t>
+  </si>
+  <si>
+    <t>*PV*</t>
   </si>
 </sst>
 </file>
@@ -729,7 +663,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -765,6 +699,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1116,36 +1051,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="11"/>
@@ -1156,9 +1091,9 @@
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>12</v>
@@ -1170,13 +1105,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>5</v>
@@ -1185,7 +1120,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>2</v>
@@ -1194,78 +1129,78 @@
         <v>7</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R3" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="W3" s="19"/>
+      <c r="X3" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
         <v>98</v>
       </c>
-      <c r="W3" s="19"/>
-      <c r="X3" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="R4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="W4" s="19"/>
       <c r="X4" s="19"/>
       <c r="Y4" s="20" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="AA4" s="20" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AB4" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="R5" t="s">
-        <v>99</v>
-      </c>
-      <c r="W5" s="29" t="s">
-        <v>45</v>
+        <v>87</v>
+      </c>
+      <c r="W5" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="X5" s="15" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="Y5" s="15">
         <v>0.2</v>
@@ -1278,52 +1213,52 @@
       </c>
       <c r="AB5" s="15"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" t="s">
+        <v>87</v>
+      </c>
+      <c r="W6" s="30"/>
+      <c r="X6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y6" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R6" t="s">
-        <v>99</v>
-      </c>
-      <c r="W6" s="29"/>
-      <c r="X6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y6" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="15">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J7" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="O7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="R7" t="s">
-        <v>99</v>
-      </c>
-      <c r="W7" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="W7" s="30"/>
       <c r="X7" s="15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="Y7" s="15">
         <v>0.03</v>
@@ -1336,23 +1271,23 @@
       </c>
       <c r="AB7" s="15"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J8" t="str">
         <f>+V21</f>
         <v>SBIORDST01</v>
       </c>
       <c r="O8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
-      </c>
-      <c r="W8" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="W8" s="30"/>
       <c r="X8" s="15" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="Y8" s="15">
         <v>0</v>
@@ -1364,26 +1299,26 @@
         <v>0</v>
       </c>
       <c r="AB8" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H9" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J9" t="str">
         <f>+V22</f>
         <v>SBIORETH01</v>
       </c>
       <c r="O9" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="R9" t="s">
-        <v>99</v>
-      </c>
-      <c r="W9" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="W9" s="30"/>
       <c r="X9" s="15" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="Y9" s="16">
         <v>0</v>
@@ -1395,26 +1330,26 @@
         <v>0</v>
       </c>
       <c r="AB9" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J10" t="str">
         <f>+U23</f>
         <v>SBIORETH03</v>
       </c>
       <c r="O10" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="R10" t="s">
-        <v>99</v>
-      </c>
-      <c r="W10" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="W10" s="30"/>
       <c r="X10" s="15" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Y10" s="16">
         <v>0</v>
@@ -1426,28 +1361,28 @@
         <v>0</v>
       </c>
       <c r="AB10" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J11" t="str">
         <f>+V28</f>
         <v>SBIORGAS01</v>
       </c>
       <c r="O11" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="R11" t="s">
-        <v>99</v>
-      </c>
-      <c r="W11" s="26" t="s">
-        <v>54</v>
+        <v>87</v>
+      </c>
+      <c r="W11" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="X11" s="15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="Y11" s="15">
         <v>30</v>
@@ -1459,39 +1394,39 @@
         <v>50</v>
       </c>
       <c r="AB11" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="W12" s="27"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="W12" s="28"/>
       <c r="X12" s="15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="Y12" s="15"/>
       <c r="Z12" s="21"/>
       <c r="AA12" s="15"/>
       <c r="AB12" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="W13" s="27"/>
+        <v>88</v>
+      </c>
+      <c r="W13" s="28"/>
       <c r="X13" s="15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="Y13" s="15"/>
       <c r="Z13" s="21"/>
       <c r="AA13" s="15"/>
       <c r="AB13" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>12</v>
@@ -1503,13 +1438,13 @@
         <v>3</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>5</v>
@@ -1518,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>2</v>
@@ -1527,17 +1462,20 @@
         <v>7</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O14" s="14" t="s">
         <v>6</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="W14" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="Q14" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="W14" s="29"/>
       <c r="X14" s="15" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="Y14" s="15"/>
       <c r="Z14" s="21">
@@ -1546,25 +1484,25 @@
       <c r="AA14" s="15"/>
       <c r="AB14" s="15"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H15">
         <f>+Z5</f>
         <v>0.6</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" t="s">
-        <v>38</v>
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>98</v>
       </c>
       <c r="O15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="W15" s="22" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="X15" s="15"/>
       <c r="Y15" s="15">
@@ -1577,86 +1515,86 @@
         <v>0</v>
       </c>
       <c r="AB15" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H16">
         <f>+Z7</f>
         <v>0.2</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="O16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H17">
         <f>+Z11</f>
         <v>43</v>
       </c>
       <c r="J17" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="O17" t="s">
-        <v>36</v>
-      </c>
-      <c r="W17" s="34"/>
-      <c r="X17" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="33"/>
-    </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="W17" s="35"/>
+      <c r="X17" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="34"/>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H18">
         <f>+Z14</f>
         <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="O18" t="s">
-        <v>36</v>
-      </c>
-      <c r="W18" s="35"/>
+        <v>24</v>
+      </c>
+      <c r="W18" s="36"/>
       <c r="X18" s="17" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Y18" s="17" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="Z18" s="23" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="AA18" s="17" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="AB18" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19">
+        <v>93</v>
+      </c>
+      <c r="H19" s="25">
         <f>10^6/Z21</f>
         <v>21739.130434782608</v>
       </c>
@@ -1665,13 +1603,13 @@
         <v>SBIORDST01</v>
       </c>
       <c r="O19" t="s">
-        <v>97</v>
-      </c>
-      <c r="W19" s="36" t="s">
-        <v>66</v>
+        <v>85</v>
+      </c>
+      <c r="W19" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="X19" s="15" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="Y19" s="15">
         <v>187</v>
@@ -1684,11 +1622,11 @@
       </c>
       <c r="AB19" s="15"/>
     </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20">
+        <v>93</v>
+      </c>
+      <c r="H20" s="25">
         <f>10^6/Z22</f>
         <v>13333.333333333334</v>
       </c>
@@ -1697,11 +1635,11 @@
         <v>SBIORETH01</v>
       </c>
       <c r="O20" t="s">
-        <v>97</v>
-      </c>
-      <c r="W20" s="37"/>
+        <v>85</v>
+      </c>
+      <c r="W20" s="38"/>
       <c r="X20" s="15" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="Y20" s="15">
         <v>137</v>
@@ -1714,11 +1652,11 @@
       </c>
       <c r="AB20" s="15"/>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21">
+        <v>93</v>
+      </c>
+      <c r="H21" s="25">
         <f>10^6/Z28</f>
         <v>7633.5877862595416</v>
       </c>
@@ -1727,16 +1665,16 @@
         <v>SBIORETH03</v>
       </c>
       <c r="O21" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="V21" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="W21" s="18" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="Y21" s="15">
         <v>36</v>
@@ -1749,11 +1687,11 @@
       </c>
       <c r="AB21" s="15"/>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22">
+        <v>93</v>
+      </c>
+      <c r="H22" s="25">
         <f>10^6/Z28</f>
         <v>7633.5877862595416</v>
       </c>
@@ -1762,16 +1700,16 @@
         <v>SBIORGAS01</v>
       </c>
       <c r="O22" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="V22" t="s">
-        <v>92</v>
-      </c>
-      <c r="W22" s="36" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="W22" s="37" t="s">
+        <v>59</v>
       </c>
       <c r="X22" s="15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="Y22" s="15">
         <v>57</v>
@@ -1784,16 +1722,16 @@
       </c>
       <c r="AB22" s="15"/>
     </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.3">
       <c r="T23" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="U23" t="s">
-        <v>93</v>
-      </c>
-      <c r="W23" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="W23" s="39"/>
       <c r="X23" s="15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Y23" s="15">
         <v>45</v>
@@ -1805,13 +1743,28 @@
         <v>61</v>
       </c>
       <c r="AB23" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="W24" s="37"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+      <c r="W24" s="38"/>
       <c r="X24" s="15" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="Y24" s="15">
         <v>92</v>
@@ -1823,15 +1776,15 @@
         <v>131</v>
       </c>
       <c r="AB24" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="W25" s="36" t="s">
-        <v>76</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="W25" s="37" t="s">
+        <v>64</v>
       </c>
       <c r="X25" s="15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="Y25" s="15">
         <v>64</v>
@@ -1843,13 +1796,13 @@
         <v>94</v>
       </c>
       <c r="AB25" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="W26" s="38"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="W26" s="39"/>
       <c r="X26" s="15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Y26" s="15">
         <v>48</v>
@@ -1861,13 +1814,13 @@
         <v>64</v>
       </c>
       <c r="AB26" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="W27" s="38"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="W27" s="39"/>
       <c r="X27" s="15" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="Y27" s="15">
         <v>132</v>
@@ -1879,19 +1832,19 @@
         <v>188</v>
       </c>
       <c r="AB27" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="V28" t="s">
-        <v>95</v>
-      </c>
-      <c r="W28" s="37"/>
+        <v>83</v>
+      </c>
+      <c r="W28" s="38"/>
       <c r="X28" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="Y28" s="15">
         <v>101</v>
@@ -1904,15 +1857,15 @@
       </c>
       <c r="AB28" s="15"/>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="W29" s="25" t="s">
-        <v>78</v>
+      <c r="W29" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="X29" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="Y29" s="15">
         <v>0</v>
@@ -1924,16 +1877,16 @@
         <v>0</v>
       </c>
       <c r="AB29" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="W30" s="25"/>
+      <c r="W30" s="26"/>
       <c r="X30" s="15" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="Y30" s="15">
         <v>0</v>
@@ -1945,16 +1898,16 @@
         <v>0</v>
       </c>
       <c r="AB30" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.3">
       <c r="K31" t="s">
         <v>8</v>
       </c>
-      <c r="W31" s="25"/>
+      <c r="W31" s="26"/>
       <c r="X31" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="Y31" s="15">
         <v>0</v>
@@ -1966,10 +1919,10 @@
         <v>0</v>
       </c>
       <c r="AB31" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C32" s="5" t="s">
         <v>1</v>
       </c>
@@ -2004,17 +1957,17 @@
         <v>10</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="W32" s="25"/>
+      <c r="W32" s="26"/>
       <c r="X32" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="Y32" s="15">
         <v>0</v>
@@ -2026,25 +1979,25 @@
         <v>0</v>
       </c>
       <c r="AB32" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C33" t="str">
         <f>"LND_perMW_SOL"</f>
         <v>LND_perMW_SOL</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J33">
         <v>2019</v>
       </c>
       <c r="K33" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="L33">
         <v>1</v>
@@ -2056,11 +2009,11 @@
         <v>5</v>
       </c>
       <c r="P33" t="s">
-        <v>104</v>
-      </c>
-      <c r="W33" s="25"/>
+        <v>92</v>
+      </c>
+      <c r="W33" s="26"/>
       <c r="X33" s="15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="Y33" s="15">
         <v>0</v>
@@ -2072,26 +2025,26 @@
         <v>0</v>
       </c>
       <c r="AB33" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="3:28" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H34" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="M34">
         <f>Z5</f>
         <v>0.6</v>
       </c>
-      <c r="W34" s="25"/>
+      <c r="W34" s="26"/>
       <c r="X34" s="15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="Y34" s="15">
         <v>0</v>
@@ -2103,25 +2056,25 @@
         <v>0</v>
       </c>
       <c r="AB34" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C35" t="str">
         <f>"LND_perMW_WND"</f>
         <v>LND_perMW_WND</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="J35">
         <v>2019</v>
       </c>
       <c r="K35" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -2133,11 +2086,11 @@
         <v>5</v>
       </c>
       <c r="P35" t="s">
-        <v>104</v>
-      </c>
-      <c r="W35" s="25"/>
+        <v>92</v>
+      </c>
+      <c r="W35" s="26"/>
       <c r="X35" s="15" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="Y35" s="15">
         <v>0</v>
@@ -2149,26 +2102,26 @@
         <v>0</v>
       </c>
       <c r="AB35" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="3:28" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H36" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="M36">
         <f>Z7</f>
         <v>0.2</v>
       </c>
-      <c r="W36" s="25"/>
+      <c r="W36" s="26"/>
       <c r="X36" s="15" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Y36" s="15">
         <v>0</v>
@@ -2180,22 +2133,22 @@
         <v>0</v>
       </c>
       <c r="AB36" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C37" t="str">
         <f>"LND_perMW_BAT"</f>
         <v>LND_perMW_BAT</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="J37">
         <v>2019</v>
       </c>
       <c r="K37" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="L37">
         <v>1</v>
@@ -2207,11 +2160,11 @@
         <v>5</v>
       </c>
       <c r="P37" t="s">
-        <v>104</v>
-      </c>
-      <c r="W37" s="25"/>
+        <v>92</v>
+      </c>
+      <c r="W37" s="26"/>
       <c r="X37" s="15" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="Y37" s="15">
         <v>0</v>
@@ -2223,23 +2176,23 @@
         <v>0</v>
       </c>
       <c r="AB37" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="3:28" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="M38">
         <f>Z11</f>
         <v>43</v>
       </c>
-      <c r="W38" s="25"/>
+      <c r="W38" s="26"/>
       <c r="X38" s="15" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="Y38" s="15">
         <v>0</v>
@@ -2251,22 +2204,22 @@
         <v>0</v>
       </c>
       <c r="AB38" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="3:28" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C39" t="str">
         <f>"LND_perMW_HPS"</f>
         <v>LND_perMW_HPS</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="J39">
         <v>2019</v>
       </c>
       <c r="K39" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -2278,15 +2231,15 @@
         <v>5</v>
       </c>
       <c r="P39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="3:28" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="3:28" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="M40">
         <f>Z14</f>
@@ -2308,479 +2261,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Land use corrected with MINLAND
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_LandUse_v1.xlsx
+++ b/SuppXLS/Scen_LandUse_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BSuleimenov\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739FEBE2-C11B-43DC-A5FF-D76B36A5C984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C118585C-9D9D-475D-A4BD-2540BF246BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="99">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -391,22 +391,22 @@
     <t>VDA_FLOP</t>
   </si>
   <si>
-    <t>ACT_EFF</t>
-  </si>
-  <si>
     <t>Other_indexes</t>
   </si>
   <si>
     <t>IE</t>
   </si>
   <si>
-    <t>PWRSOL</t>
-  </si>
-  <si>
     <t>*PV*</t>
   </si>
   <si>
     <t>UC_T</t>
+  </si>
+  <si>
+    <t>ACT_BND</t>
+  </si>
+  <si>
+    <t>MINLAND</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>5</v>
@@ -1157,7 +1157,7 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O4" t="s">
         <v>23</v>
@@ -1444,7 +1444,7 @@
         <v>19</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>5</v>
@@ -1471,7 +1471,7 @@
         <v>17</v>
       </c>
       <c r="Q14" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W14" s="29"/>
       <c r="X14" s="15" t="s">
@@ -1496,7 +1496,7 @@
         <v>24</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O15" t="s">
         <v>23</v>
@@ -1748,19 +1748,16 @@
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="E24">
+        <v>2018</v>
       </c>
       <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>23</v>
+        <v>120</v>
+      </c>
+      <c r="J24" t="s">
+        <v>98</v>
       </c>
       <c r="W24" s="38"/>
       <c r="X24" s="15" t="s">
@@ -1780,6 +1777,18 @@
       </c>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25">
+        <v>2040</v>
+      </c>
+      <c r="H25">
+        <v>150</v>
+      </c>
+      <c r="J25" t="s">
+        <v>98</v>
+      </c>
       <c r="W25" s="37" t="s">
         <v>63</v>
       </c>
@@ -1800,6 +1809,18 @@
       </c>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>98</v>
+      </c>
       <c r="W26" s="39"/>
       <c r="X26" s="15" t="s">
         <v>60</v>
@@ -1903,7 +1924,7 @@
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="K31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W31" s="26"/>
       <c r="X31" s="15" t="s">

</xml_diff>

<commit_message>
LandUse of wind/solar - new design
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_LandUse_v1.xlsx
+++ b/SuppXLS/Scen_LandUse_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BSuleimenov\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C118585C-9D9D-475D-A4BD-2540BF246BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7951FD8B-48F9-4BA6-966E-FFA87120D483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{53508571-8973-4AE0-A8EA-12F57BF1421B}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{53508571-8973-4AE0-A8EA-12F57BF1421B}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -127,9 +127,6 @@
     <t>UC_CAP</t>
   </si>
   <si>
-    <t>UC_FLO</t>
-  </si>
-  <si>
     <t>Attribute</t>
   </si>
   <si>
@@ -169,13 +166,7 @@
     <t>~TFM_TOPINS</t>
   </si>
   <si>
-    <t>POW_LAND</t>
-  </si>
-  <si>
     <t>ELE</t>
-  </si>
-  <si>
-    <t>ELCSOL</t>
   </si>
   <si>
     <t>*WIN*ON*</t>
@@ -400,13 +391,28 @@
     <t>*PV*</t>
   </si>
   <si>
-    <t>UC_T</t>
-  </si>
-  <si>
     <t>ACT_BND</t>
   </si>
   <si>
     <t>MINLAND</t>
+  </si>
+  <si>
+    <t>UC_ACT</t>
+  </si>
+  <si>
+    <t>SOLLAND</t>
+  </si>
+  <si>
+    <t>WINDLAND</t>
+  </si>
+  <si>
+    <t>BATLAND</t>
+  </si>
+  <si>
+    <t>PUMPLAND</t>
+  </si>
+  <si>
+    <t>~UC_T</t>
   </si>
 </sst>
 </file>
@@ -762,6 +768,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -1049,38 +1059,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="11"/>
@@ -1091,27 +1101,27 @@
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>19</v>
-      </c>
       <c r="H3" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>5</v>
@@ -1120,7 +1130,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>2</v>
@@ -1129,78 +1139,74 @@
         <v>7</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="W3" s="19"/>
       <c r="X3" s="31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Y3" s="31"/>
       <c r="Z3" s="31"/>
       <c r="AA3" s="31"/>
       <c r="AB3" s="31"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>95</v>
+        <v>83</v>
+      </c>
+      <c r="J4" t="str">
+        <f>+V21</f>
+        <v>SBIORDST01</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="R4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="W4" s="19"/>
       <c r="X4" s="19"/>
       <c r="Y4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z4" s="23" t="s">
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="str">
+        <f>+V22</f>
+        <v>SBIORETH01</v>
+      </c>
+      <c r="O5" t="s">
+        <v>81</v>
+      </c>
+      <c r="R5" t="s">
+        <v>83</v>
+      </c>
+      <c r="W5" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AA4" s="20" t="s">
+      <c r="X5" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="AB4" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" t="s">
-        <v>86</v>
-      </c>
-      <c r="W5" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="X5" s="15" t="s">
-        <v>33</v>
       </c>
       <c r="Y5" s="15">
         <v>0.2</v>
@@ -1213,22 +1219,23 @@
       </c>
       <c r="AB5" s="15"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="J6" t="str">
+        <f>+U23</f>
+        <v>SBIORETH03</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="R6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="W6" s="30"/>
       <c r="X6" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Y6" s="15">
         <v>0</v>
@@ -1240,25 +1247,26 @@
         <v>0</v>
       </c>
       <c r="AB6" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="J7" t="str">
+        <f>+V28</f>
+        <v>SBIORGAS01</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="R7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="W7" s="30"/>
       <c r="X7" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Y7" s="15">
         <v>0.03</v>
@@ -1271,23 +1279,10 @@
       </c>
       <c r="AB7" s="15"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J8" t="str">
-        <f>+V21</f>
-        <v>SBIORDST01</v>
-      </c>
-      <c r="O8" t="s">
-        <v>84</v>
-      </c>
-      <c r="R8" t="s">
-        <v>86</v>
-      </c>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="W8" s="30"/>
       <c r="X8" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y8" s="15">
         <v>0</v>
@@ -1299,26 +1294,16 @@
         <v>0</v>
       </c>
       <c r="AB8" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" t="str">
-        <f>+V22</f>
-        <v>SBIORETH01</v>
-      </c>
-      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="R9" t="s">
-        <v>86</v>
       </c>
       <c r="W9" s="30"/>
       <c r="X9" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Y9" s="16">
         <v>0</v>
@@ -1330,26 +1315,61 @@
         <v>0</v>
       </c>
       <c r="AB9" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J10" t="str">
-        <f>+U23</f>
-        <v>SBIORETH03</v>
-      </c>
-      <c r="O10" t="s">
-        <v>84</v>
-      </c>
-      <c r="R10" t="s">
-        <v>86</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="24" t="s">
+        <v>90</v>
       </c>
       <c r="W10" s="30"/>
       <c r="X10" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Y10" s="16">
         <v>0</v>
@@ -1361,28 +1381,29 @@
         <v>0</v>
       </c>
       <c r="AB10" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="25">
+        <f>10^6/Z21</f>
+        <v>21739.130434782608</v>
+      </c>
+      <c r="J11" t="str">
+        <f>J4</f>
+        <v>SBIORDST01</v>
+      </c>
+      <c r="O11" t="s">
+        <v>81</v>
+      </c>
+      <c r="W11" s="27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" t="str">
-        <f>+V28</f>
-        <v>SBIORGAS01</v>
-      </c>
-      <c r="O11" t="s">
-        <v>84</v>
-      </c>
-      <c r="R11" t="s">
-        <v>86</v>
-      </c>
-      <c r="W11" s="27" t="s">
-        <v>41</v>
-      </c>
       <c r="X11" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Y11" s="15">
         <v>30</v>
@@ -1394,88 +1415,79 @@
         <v>50</v>
       </c>
       <c r="AB11" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="25">
+        <f>10^6/Z22</f>
+        <v>13333.333333333334</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ref="J12:J14" si="0">J5</f>
+        <v>SBIORETH01</v>
+      </c>
+      <c r="O12" t="s">
+        <v>81</v>
+      </c>
       <c r="W12" s="28"/>
       <c r="X12" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Y12" s="15"/>
       <c r="Z12" s="21"/>
       <c r="AA12" s="15"/>
       <c r="AB12" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
-        <v>87</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="25">
+        <f>10^6/Z28</f>
+        <v>7633.5877862595416</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>SBIORETH03</v>
+      </c>
+      <c r="O13" t="s">
+        <v>81</v>
       </c>
       <c r="W13" s="28"/>
       <c r="X13" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Y13" s="15"/>
       <c r="Z13" s="21"/>
       <c r="AA13" s="15"/>
       <c r="AB13" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q14" s="24" t="s">
-        <v>93</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="25">
+        <f>10^6/Z28</f>
+        <v>7633.5877862595416</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>SBIORGAS01</v>
+      </c>
+      <c r="O14" t="s">
+        <v>81</v>
       </c>
       <c r="W14" s="29"/>
       <c r="X14" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Y14" s="15"/>
       <c r="Z14" s="21">
@@ -1484,25 +1496,9 @@
       <c r="AA14" s="15"/>
       <c r="AB14" s="15"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15">
-        <f>+Z5</f>
-        <v>0.6</v>
-      </c>
-      <c r="I15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" t="s">
-        <v>95</v>
-      </c>
-      <c r="O15" t="s">
-        <v>23</v>
-      </c>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="W15" s="22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="X15" s="15"/>
       <c r="Y15" s="15">
@@ -1515,101 +1511,81 @@
         <v>0</v>
       </c>
       <c r="AB15" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="E16">
+        <v>2018</v>
       </c>
       <c r="H16">
-        <f>+Z7</f>
-        <v>0.2</v>
-      </c>
-      <c r="I16" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="E17">
+        <v>2040</v>
       </c>
       <c r="H17">
-        <f>+Z11</f>
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="J17" t="s">
-        <v>77</v>
-      </c>
-      <c r="O17" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="W17" s="35"/>
       <c r="X17" s="32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Y17" s="33"/>
       <c r="Z17" s="33"/>
       <c r="AA17" s="33"/>
       <c r="AB17" s="34"/>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
       <c r="H18">
-        <f>+Z14</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
-      </c>
-      <c r="O18" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="W18" s="36"/>
       <c r="X18" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB18" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="W19" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="X19" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="Y18" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z18" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB18" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="25">
-        <f>10^6/Z21</f>
-        <v>21739.130434782608</v>
-      </c>
-      <c r="J19" t="str">
-        <f>J8</f>
-        <v>SBIORDST01</v>
-      </c>
-      <c r="O19" t="s">
-        <v>84</v>
-      </c>
-      <c r="W19" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="X19" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="Y19" s="15">
         <v>187</v>
@@ -1622,24 +1598,13 @@
       </c>
       <c r="AB19" s="15"/>
     </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="25">
-        <f>10^6/Z22</f>
-        <v>13333.333333333334</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" ref="J20:J22" si="0">J9</f>
-        <v>SBIORETH01</v>
-      </c>
-      <c r="O20" t="s">
-        <v>84</v>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>19</v>
       </c>
       <c r="W20" s="38"/>
       <c r="X20" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Y20" s="15">
         <v>137</v>
@@ -1652,29 +1617,18 @@
       </c>
       <c r="AB20" s="15"/>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="25">
-        <f>10^6/Z28</f>
-        <v>7633.5877862595416</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="0"/>
-        <v>SBIORETH03</v>
-      </c>
-      <c r="O21" t="s">
-        <v>84</v>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="V21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="W21" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Y21" s="15">
         <v>36</v>
@@ -1687,29 +1641,18 @@
       </c>
       <c r="AB21" s="15"/>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="25">
-        <f>10^6/Z28</f>
-        <v>7633.5877862595416</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="0"/>
-        <v>SBIORGAS01</v>
-      </c>
-      <c r="O22" t="s">
-        <v>84</v>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="V22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="W22" s="37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="X22" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Y22" s="15">
         <v>57</v>
@@ -1722,16 +1665,19 @@
       </c>
       <c r="AB22" s="15"/>
     </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>100</v>
+      </c>
       <c r="T23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="U23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="W23" s="39"/>
       <c r="X23" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Y23" s="15">
         <v>45</v>
@@ -1743,25 +1689,55 @@
         <v>61</v>
       </c>
       <c r="AB23" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24">
-        <v>2018</v>
-      </c>
-      <c r="H24">
-        <v>120</v>
-      </c>
-      <c r="J24" t="s">
-        <v>98</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="W24" s="38"/>
       <c r="X24" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Y24" s="15">
         <v>92</v>
@@ -1773,27 +1749,43 @@
         <v>131</v>
       </c>
       <c r="AB24" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <f>"LND_perMW_SOL"</f>
+        <v>LND_perMW_SOL</v>
+      </c>
       <c r="D25" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25">
-        <v>2040</v>
-      </c>
-      <c r="H25">
-        <v>150</v>
-      </c>
-      <c r="J25" t="s">
-        <v>98</v>
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25">
+        <v>2019</v>
+      </c>
+      <c r="K25" t="s">
+        <v>87</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
+      </c>
+      <c r="P25" t="s">
+        <v>88</v>
       </c>
       <c r="W25" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="X25" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Y25" s="15">
         <v>64</v>
@@ -1805,25 +1797,20 @@
         <v>94</v>
       </c>
       <c r="AB25" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>5</v>
-      </c>
-      <c r="J26" t="s">
-        <v>98</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M26">
+        <f>-Z5*1000</f>
+        <v>-600</v>
       </c>
       <c r="W26" s="39"/>
       <c r="X26" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Y26" s="15">
         <v>48</v>
@@ -1835,13 +1822,41 @@
         <v>64</v>
       </c>
       <c r="AB26" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C27" t="str">
+        <f>"LND_perMW_WND"</f>
+        <v>LND_perMW_WND</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27">
+        <v>2019</v>
+      </c>
+      <c r="K27" t="s">
+        <v>87</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="P27" t="s">
+        <v>88</v>
+      </c>
       <c r="W27" s="39"/>
       <c r="X27" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Y27" s="15">
         <v>132</v>
@@ -1853,19 +1868,23 @@
         <v>188</v>
       </c>
       <c r="AB27" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="M28">
+        <f>-Z7*1000</f>
+        <v>-200</v>
       </c>
       <c r="V28" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="W28" s="38"/>
       <c r="X28" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Y28" s="15">
         <v>101</v>
@@ -1878,15 +1897,37 @@
       </c>
       <c r="AB28" s="15"/>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
-        <v>0</v>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C29" t="str">
+        <f>"LND_perMW_BAT"</f>
+        <v>LND_perMW_BAT</v>
+      </c>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29">
+        <v>2019</v>
+      </c>
+      <c r="K29" t="s">
+        <v>87</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>5</v>
+      </c>
+      <c r="P29" t="s">
+        <v>88</v>
       </c>
       <c r="W29" s="26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="X29" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Y29" s="15">
         <v>0</v>
@@ -1898,16 +1939,20 @@
         <v>0</v>
       </c>
       <c r="AB29" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C30" s="7" t="s">
-        <v>12</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="M30">
+        <f>-Z11*1000</f>
+        <v>-43000</v>
       </c>
       <c r="W30" s="26"/>
       <c r="X30" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Y30" s="15">
         <v>0</v>
@@ -1919,16 +1964,38 @@
         <v>0</v>
       </c>
       <c r="AB30" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C31" t="str">
+        <f>"LND_perMW_HPS"</f>
+        <v>LND_perMW_HPS</v>
+      </c>
+      <c r="E31" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31">
+        <v>2019</v>
+      </c>
       <c r="K31" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="P31" t="s">
+        <v>88</v>
       </c>
       <c r="W31" s="26"/>
       <c r="X31" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y31" s="15">
         <v>0</v>
@@ -1940,55 +2007,20 @@
         <v>0</v>
       </c>
       <c r="AB31" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>99</v>
+      </c>
+      <c r="M32">
+        <f>-Z14*1000</f>
+        <v>-10000</v>
       </c>
       <c r="W32" s="26"/>
       <c r="X32" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Y32" s="15">
         <v>0</v>
@@ -2000,41 +2032,13 @@
         <v>0</v>
       </c>
       <c r="AB32" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C33" t="str">
-        <f>"LND_perMW_SOL"</f>
-        <v>LND_perMW_SOL</v>
-      </c>
-      <c r="D33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33">
-        <v>2019</v>
-      </c>
-      <c r="K33" t="s">
-        <v>90</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>5</v>
-      </c>
-      <c r="P33" t="s">
-        <v>91</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W33" s="26"/>
       <c r="X33" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Y33" s="15">
         <v>0</v>
@@ -2046,26 +2050,13 @@
         <v>0</v>
       </c>
       <c r="AB33" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" t="s">
-        <v>23</v>
-      </c>
-      <c r="M34">
-        <f>Z5</f>
-        <v>0.6</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W34" s="26"/>
       <c r="X34" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Y34" s="15">
         <v>0</v>
@@ -2077,41 +2068,13 @@
         <v>0</v>
       </c>
       <c r="AB34" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C35" t="str">
-        <f>"LND_perMW_WND"</f>
-        <v>LND_perMW_WND</v>
-      </c>
-      <c r="D35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
-      </c>
-      <c r="J35">
-        <v>2019</v>
-      </c>
-      <c r="K35" t="s">
-        <v>90</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>5</v>
-      </c>
-      <c r="P35" t="s">
-        <v>91</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W35" s="26"/>
       <c r="X35" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Y35" s="15">
         <v>0</v>
@@ -2123,26 +2086,13 @@
         <v>0</v>
       </c>
       <c r="AB35" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36">
-        <f>Z7</f>
-        <v>0.2</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W36" s="26"/>
       <c r="X36" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Y36" s="15">
         <v>0</v>
@@ -2154,38 +2104,13 @@
         <v>0</v>
       </c>
       <c r="AB36" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C37" t="str">
-        <f>"LND_perMW_BAT"</f>
-        <v>LND_perMW_BAT</v>
-      </c>
-      <c r="E37" t="s">
-        <v>77</v>
-      </c>
-      <c r="J37">
-        <v>2019</v>
-      </c>
-      <c r="K37" t="s">
-        <v>90</v>
-      </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>5</v>
-      </c>
-      <c r="P37" t="s">
-        <v>91</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W37" s="26"/>
       <c r="X37" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Y37" s="15">
         <v>0</v>
@@ -2197,23 +2122,13 @@
         <v>0</v>
       </c>
       <c r="AB37" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" t="s">
-        <v>23</v>
-      </c>
-      <c r="M38">
-        <f>Z11</f>
-        <v>43</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W38" s="26"/>
       <c r="X38" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Y38" s="15">
         <v>0</v>
@@ -2225,46 +2140,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="C39" t="str">
-        <f>"LND_perMW_HPS"</f>
-        <v>LND_perMW_HPS</v>
-      </c>
-      <c r="E39" t="s">
-        <v>78</v>
-      </c>
-      <c r="J39">
-        <v>2019</v>
-      </c>
-      <c r="K39" t="s">
-        <v>90</v>
-      </c>
-      <c r="L39">
-        <v>1</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>5</v>
-      </c>
-      <c r="P39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="3:28" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" t="s">
-        <v>23</v>
-      </c>
-      <c r="M40">
-        <f>Z14</f>
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>